<commit_message>
Control de pst cambio del backup a disco Extraible
</commit_message>
<xml_diff>
--- a/AdministradorTI/archivos/plantillas_excel/BACKUP_BITACORA.xlsx
+++ b/AdministradorTI/archivos/plantillas_excel/BACKUP_BITACORA.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LEONARD\python-dev\incasur-projecto\AdministradorTI\archivos\plantillas_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1F72EFA-18FB-4A00-B759-630F0D1DFDE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C2B484C-8142-4575-825F-F45CF71BA7E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{96A09CA5-C5A8-4FC0-BB8E-6EA2B261C5E3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>FORMATO DE BITACORA DE BACKUPS</t>
   </si>
@@ -61,6 +61,12 @@
   </si>
   <si>
     <t>Puesto de Colaborador :</t>
+  </si>
+  <si>
+    <t>Personal TI Encargado</t>
+  </si>
+  <si>
+    <t>Colaborador</t>
   </si>
 </sst>
 </file>
@@ -107,15 +113,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -214,23 +226,32 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thick">
         <color indexed="64"/>
       </left>
       <right/>
       <top/>
-      <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thick">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -239,18 +260,18 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="thick">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right/>
-      <top style="thick">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thick">
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -259,21 +280,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -282,7 +306,7 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -303,6 +327,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -310,64 +346,71 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -432,245 +475,6 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>705548</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>98967</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>791273</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>98967</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="3" name="Conector recto 50">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CFD985AF-03CC-4D24-B496-866468C0511B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="705548" y="3425747"/>
-          <a:ext cx="1617159" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="19050"/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>358140</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>108585</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>108585</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="4" name="Conector recto 51">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7DD0B609-0E07-4623-97E5-781518290891}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3268980" y="3453765"/>
-          <a:ext cx="1680210" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="19050"/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>695324</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>117831</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>175259</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>194031</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="CuadroTexto 52">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5FFAC632-0579-4020-9125-D840432CE153}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="695324" y="3444611"/>
-          <a:ext cx="1803106" cy="273205"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="es-PE" sz="1100"/>
-            <a:t>Personal</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-PE" sz="1100" baseline="0"/>
-            <a:t> de TI Encargado</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="CuadroTexto 53">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7024C14D-040B-4C10-AC77-7315F341A554}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4507230" y="3469005"/>
-          <a:ext cx="1040130" cy="255270"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="es-PE" sz="1100"/>
-            <a:t>Colaborador </a:t>
-          </a:r>
-          <a:endParaRPr lang="es-PE" sz="1100" baseline="0"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -971,10 +775,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1C976F5-74F0-4950-B306-3882852B8852}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10:H10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11:H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -983,218 +787,251 @@
     <col min="4" max="4" width="8.5546875" customWidth="1"/>
     <col min="5" max="5" width="6.33203125" customWidth="1"/>
     <col min="6" max="6" width="11.88671875" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" customWidth="1"/>
+    <col min="8" max="8" width="7.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="18" t="s">
+    <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-    </row>
-    <row r="3" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="17"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-    </row>
-    <row r="4" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="17"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-    </row>
-    <row r="5" spans="1:8" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="17"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="19" t="s">
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:12" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="23"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20" t="s">
+      <c r="D5" s="4"/>
+      <c r="E5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-    </row>
-    <row r="6" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="17"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="4" t="s">
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+    </row>
+    <row r="6" spans="1:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="23"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="7">
+      <c r="D6" s="6"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="8">
         <f ca="1">NOW()</f>
-        <v>46052.505213888886</v>
-      </c>
-      <c r="G6" s="8"/>
-      <c r="H6" s="9"/>
-    </row>
-    <row r="7" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="15" t="s">
+        <v>46069.409286226852</v>
+      </c>
+      <c r="G6" s="9"/>
+      <c r="H6" s="10"/>
+    </row>
+    <row r="7" spans="1:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-    </row>
-    <row r="8" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="15" t="s">
+      <c r="B7" s="21"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+    </row>
+    <row r="8" spans="1:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-    </row>
-    <row r="9" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="15" t="s">
+      <c r="B8" s="21"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+    </row>
+    <row r="9" spans="1:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="17" t="s">
+      <c r="B9" s="21"/>
+      <c r="C9" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-    </row>
-    <row r="10" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="10" t="s">
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="J9" s="36"/>
+      <c r="K9" s="36"/>
+      <c r="L9" s="36"/>
+    </row>
+    <row r="10" spans="1:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="14" t="s">
+      <c r="B10" s="12"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="13"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="13"/>
-    </row>
-    <row r="11" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="22" t="s">
+      <c r="F10" s="14"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="14"/>
+      <c r="J10" s="36"/>
+      <c r="K10" s="36"/>
+      <c r="L10" s="36"/>
+    </row>
+    <row r="11" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="23"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="30"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="24"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="33"/>
-    </row>
-    <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="26"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="34"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="36"/>
-    </row>
-    <row r="14" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
+      <c r="B11" s="17"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="28"/>
+      <c r="J11" s="36"/>
+      <c r="K11" s="36"/>
+      <c r="L11" s="36"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="18"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="30"/>
+      <c r="J12" s="36"/>
+      <c r="K12" s="36"/>
+      <c r="L12" s="36"/>
+    </row>
+    <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="18"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="30"/>
+      <c r="J13" s="36"/>
+      <c r="K13" s="36"/>
+      <c r="L13" s="36"/>
+    </row>
+    <row r="14" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-    </row>
-    <row r="15" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-    </row>
-    <row r="16" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-    </row>
-    <row r="17" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-    </row>
-    <row r="18" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-    </row>
-    <row r="19" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-    </row>
-    <row r="20" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="35"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="37"/>
+      <c r="J14" s="36"/>
+      <c r="K14" s="36"/>
+      <c r="L14" s="36"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="40"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="36"/>
+      <c r="J15" s="36"/>
+      <c r="K15" s="36"/>
+      <c r="L15" s="36"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="40"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="38"/>
+      <c r="J16" s="36"/>
+      <c r="K16" s="36"/>
+      <c r="L16" s="36"/>
+    </row>
+    <row r="17" spans="1:12" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="40"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="38"/>
+      <c r="J17" s="36"/>
+      <c r="K17" s="36"/>
+      <c r="L17" s="36"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" s="41"/>
+      <c r="B18" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="25"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" s="25"/>
+      <c r="H18" s="43"/>
+    </row>
+    <row r="19" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="42"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="44"/>
+      <c r="I19" s="36"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1205,11 +1042,16 @@
       <c r="H20" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="21">
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:H9"/>
+    <mergeCell ref="A2:B6"/>
+    <mergeCell ref="B18:C19"/>
+    <mergeCell ref="F18:G19"/>
+    <mergeCell ref="A14:H17"/>
     <mergeCell ref="C2:H4"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="E5:H5"/>
-    <mergeCell ref="A14:H19"/>
     <mergeCell ref="C6:E6"/>
     <mergeCell ref="F6:H6"/>
     <mergeCell ref="A10:B10"/>
@@ -1222,9 +1064,6 @@
     <mergeCell ref="C7:H7"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="C8:H8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:H9"/>
-    <mergeCell ref="A2:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>

</xml_diff>